<commit_message>
update to query, include AggregationIntervalUnitCV
</commit_message>
<xml_diff>
--- a/20221025 Summary of SSPS/Summary Results.xlsx
+++ b/20221025 Summary of SSPS/Summary Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\WaDE-Side-Projects\20221025 Summary of SSPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A812844E-9487-4D78-9F3A-3D041629CCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A792A5-5AD5-4138-BAFF-93F31382D3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{AE5C7255-74E0-499C-9957-60819E71160E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="93">
   <si>
     <t>State</t>
   </si>
@@ -303,7 +303,22 @@
     <t>----|----|----</t>
   </si>
   <si>
-    <t>----|----|---- |----</t>
+    <t xml:space="preserve">AggregationIntervalUnitCV </t>
+  </si>
+  <si>
+    <t>numUniqueYears</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>----|----|---- |----|----|----</t>
   </si>
 </sst>
 </file>
@@ -685,7 +700,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J18:J19"/>
+      <selection activeCell="J27" sqref="J26:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +764,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="H3" t="str">
-        <f>A2&amp;"|"&amp;B2&amp;"|"&amp;C2</f>
+        <f t="shared" ref="H3:H8" si="0">A2&amp;"|"&amp;B2&amp;"|"&amp;C2</f>
         <v>CA|POU|3960</v>
       </c>
     </row>
@@ -764,7 +779,7 @@
         <v>535</v>
       </c>
       <c r="H4" t="str">
-        <f>A3&amp;"|"&amp;B3&amp;"|"&amp;C3</f>
+        <f t="shared" si="0"/>
         <v>NJ|POU|472</v>
       </c>
     </row>
@@ -779,7 +794,7 @@
         <v>4035</v>
       </c>
       <c r="H5" t="str">
-        <f>A4&amp;"|"&amp;B4&amp;"|"&amp;C4</f>
+        <f t="shared" si="0"/>
         <v>NM|POD|535</v>
       </c>
     </row>
@@ -794,7 +809,7 @@
         <v>4926</v>
       </c>
       <c r="H6" t="str">
-        <f>A5&amp;"|"&amp;B5&amp;"|"&amp;C5</f>
+        <f t="shared" si="0"/>
         <v>TX|POU|4035</v>
       </c>
     </row>
@@ -809,13 +824,13 @@
         <v>541</v>
       </c>
       <c r="H7" t="str">
-        <f>A6&amp;"|"&amp;B6&amp;"|"&amp;C6</f>
+        <f t="shared" si="0"/>
         <v>UT|POD|4926</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H8" t="str">
-        <f>A7&amp;"|"&amp;B7&amp;"|"&amp;C7</f>
+        <f t="shared" si="0"/>
         <v>UT|POU|541</v>
       </c>
     </row>
@@ -2188,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC99448C-F171-45FF-B693-ABF57F178EFE}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H7"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2200,128 +2215,170 @@
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="str">
-        <f>A1&amp;"|"&amp;B1&amp;"|"&amp;C1&amp;"|"&amp;D1</f>
-        <v>State|minYear|maxYear|TimeRange_Yrs</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="str">
+        <f>A1&amp;"|"&amp;B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1&amp;"|"&amp;F1</f>
+        <v>State|AggregationIntervalUnitCV |minYear|maxYear|numUniqueYears|TimeRange_Yrs</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2">
         <v>2013</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2016</v>
       </c>
-      <c r="D2">
-        <f>C2-B2</f>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>D2-C2</f>
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3">
         <v>1990</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2018</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">C3-B3</f>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="0">D3-C3</f>
         <v>28</v>
       </c>
-      <c r="H3" t="str">
-        <f>A2&amp;"|"&amp;B2&amp;"|"&amp;C2&amp;"|"&amp;D2</f>
-        <v>CA|2013|2016|3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="str">
+        <f>A2&amp;"|"&amp;B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2&amp;"|"&amp;F2</f>
+        <v>CA|Monthly|2013|2016|4|3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4">
         <v>2010</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2015</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" ref="H4:H7" si="1">A3&amp;"|"&amp;B3&amp;"|"&amp;C3&amp;"|"&amp;D3</f>
-        <v>NJ|1990|2018|28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I7" si="1">A3&amp;"|"&amp;B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3&amp;"|"&amp;F3</f>
+        <v>NJ|Monthly|1990|2018|29|28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5">
         <v>1955</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2021</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>67</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>NM|2010|2015|5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>NM|Annual|2010|2015|2|5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
         <v>1957</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2020</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>TX|1955|2021|66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" t="str">
+        <v>TX|Monthly|1955|2021|67|66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>UT|1957|2020|63</v>
-      </c>
+        <v>UT|Year|1957|2020|64|63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update. changed count to include unique time series entries.
</commit_message>
<xml_diff>
--- a/20221025 Summary of SSPS/Summary Results.xlsx
+++ b/20221025 Summary of SSPS/Summary Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\WaDE-Side-Projects\20221025 Summary of SSPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A792A5-5AD5-4138-BAFF-93F31382D3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33434B5E-6A6A-43AB-8F37-C432950ED575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{AE5C7255-74E0-499C-9957-60819E71160E}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12456" xr2:uid="{AE5C7255-74E0-499C-9957-60819E71160E}"/>
   </bookViews>
   <sheets>
     <sheet name="POD v POU" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t xml:space="preserve">AggregationIntervalUnitCV </t>
   </si>
   <si>
-    <t>numUniqueYears</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>----|----|---- |----|----|----</t>
+  </si>
+  <si>
+    <t>numUniqueTimeSeriesEntries</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J26:J27"/>
+      <selection activeCell="F15" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2206,7 +2206,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,7 +2215,7 @@
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2234,14 +2234,14 @@
         <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
       <c r="I1" t="str">
         <f>A1&amp;"|"&amp;B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1&amp;"|"&amp;F1</f>
-        <v>State|AggregationIntervalUnitCV |minYear|maxYear|numUniqueYears|TimeRange_Yrs</v>
+        <v>State|AggregationIntervalUnitCV |minYear|maxYear|numUniqueTimeSeriesEntries|TimeRange_Yrs</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -2249,7 +2249,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2">
         <v>2013</v>
@@ -2258,14 +2258,14 @@
         <v>2016</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <f>D2-C2</f>
         <v>3</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2273,7 +2273,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>1990</v>
@@ -2282,7 +2282,7 @@
         <v>2018</v>
       </c>
       <c r="E3">
-        <v>29</v>
+        <v>348</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F6" si="0">D3-C3</f>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="I3" t="str">
         <f>A2&amp;"|"&amp;B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2&amp;"|"&amp;F2</f>
-        <v>CA|Monthly|2013|2016|4|3</v>
+        <v>CA|Monthly|2013|2016|48|3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -2298,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>2010</v>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I7" si="1">A3&amp;"|"&amp;B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3&amp;"|"&amp;F3</f>
-        <v>NJ|Monthly|1990|2018|29|28</v>
+        <v>NJ|Monthly|1990|2018|348|28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2323,7 +2323,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <v>1955</v>
@@ -2332,7 +2332,7 @@
         <v>2021</v>
       </c>
       <c r="E5">
-        <v>67</v>
+        <v>335</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -2348,7 +2348,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6">
         <v>1957</v>
@@ -2357,7 +2357,7 @@
         <v>2020</v>
       </c>
       <c r="E6">
-        <v>64</v>
+        <v>746</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
@@ -2365,13 +2365,13 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>TX|Monthly|1955|2021|67|66</v>
+        <v>TX|Monthly|1955|2021|335|66</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>UT|Year|1957|2020|64|63</v>
+        <v>UT|Year|1957|2020|746|63</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>